<commit_message>
refactor: update location names to be anonymous and add a Jupyter Notebook for SNR heatmap
</commit_message>
<xml_diff>
--- a/dataset/results_for_t_test.xlsx
+++ b/dataset/results_for_t_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selinbac/Desktop/UCSB/Accelerate/Data/01 Round Robin GC Results/last_AUC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dongjae/Dropbox/0.Dongjae/04.SUNCAT@SLAC,Standford(2402~)/231128_research/240602_ML_codes/PyCatRobin/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966D1643-C54E-724E-AF7A-C75227DE5D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C04F032-3D37-864A-AC31-8F797604351B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35880" yWindow="100" windowWidth="29400" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,102 +110,6 @@
     <t>Selectivity to CO (%) | AUC</t>
   </si>
   <si>
-    <t>2p0_RhWI_0p02_500C_20250331_PSURight.xlsx</t>
-  </si>
-  <si>
-    <t>0p3_RhNP_0p0197mg_500C_20250211_Cargnello1.xlsx</t>
-  </si>
-  <si>
-    <t>0p3_RhWI_0p02mg_500C_20250331_SLAC1.xlsx</t>
-  </si>
-  <si>
-    <t>0p1_RhWI_0p02mg_500C_20250319_UCSBRR.xlsx</t>
-  </si>
-  <si>
-    <t>0p3_RhWI_0p0199mg_500C_20250415_SLAC1.xlsx</t>
-  </si>
-  <si>
-    <t>2_RhWI_0p0202mg_500C_20250317_Cargnello1.xlsx</t>
-  </si>
-  <si>
-    <t>0p3_RhWI_0p0204mg_500C_20250421_SLAC1.xlsx</t>
-  </si>
-  <si>
-    <t>2_RhWI_0p027_600C_20250422_PSURight.xlsx</t>
-  </si>
-  <si>
-    <t>0p3_RhWI_0p0207_500C_20250315_PSURight.xlsx</t>
-  </si>
-  <si>
-    <t>2_RhWI_0p02mg_400C_20250422_SLAC1.xlsx</t>
-  </si>
-  <si>
-    <t>0p3_RhNP_0p0201mg_500C_20250312_UCSBRR.xlsx</t>
-  </si>
-  <si>
-    <t>0p3_RhWI_0p02mg_500C_20250312_Cargnello1.xlsx</t>
-  </si>
-  <si>
-    <t>2_RhWI_0p02mg_500C_20250417_SLAC1.xlsx</t>
-  </si>
-  <si>
-    <t>2_RhWI_0p0204mg_400C_20250324_Cargnello1.xlsx</t>
-  </si>
-  <si>
-    <t>0p3_RhWI_0p0201mg_500C_20250311_UCSBRR.xlsx</t>
-  </si>
-  <si>
-    <t>0p3_RhNP_0p0201mg_500C_20250207_Cargnello1.xlsx</t>
-  </si>
-  <si>
-    <t>2_RhWI_0p02mg_400C_20250306_UCSBRR.xlsx</t>
-  </si>
-  <si>
-    <t>0p1_RhWI_0p02_500C_20250414_PSURight.xlsx</t>
-  </si>
-  <si>
-    <t>2_RhWI_0p02mg_600C_20250318_UCSBRR.xlsx</t>
-  </si>
-  <si>
-    <t>2_RhWI_0p02mg_500C_20250307_UCSBRR.xlsx</t>
-  </si>
-  <si>
-    <t>0p1_RhWI_0p02mg_500C_20250418_SLAC1.xlsx</t>
-  </si>
-  <si>
-    <t>2_RhWI_0p02mg_600C_20250326_Cargnello1.xlsx</t>
-  </si>
-  <si>
-    <t>2_RhWI_0p01824_500C_20250401_PSURight.xlsx</t>
-  </si>
-  <si>
-    <t>2_RhWI_0p02mg_600C_20250423_SLAC1.xlsx</t>
-  </si>
-  <si>
-    <t>0p1_RhWI_0p02mg_500C_20250314_UCSBRR.xlsx</t>
-  </si>
-  <si>
-    <t>0p1_RhWI_0p02mg_500C_20250314_Cargnello1.xlsx</t>
-  </si>
-  <si>
-    <t>0p3_RhNP_0p0201mg_500C_20250424_SLAC1.xlsx</t>
-  </si>
-  <si>
-    <t>0p1_RhWI_0p02mg_500C_20250317_UCSBRR.xlsx</t>
-  </si>
-  <si>
-    <t>2_RhWI_0p021_400C_20250425_PSURight.xlsx</t>
-  </si>
-  <si>
-    <t>2_RhWI_0p02_500C_20250403_PSURight.xlsx</t>
-  </si>
-  <si>
-    <t>0p3_RhNP_0p0199mg_500C_20250212_Cargnello1.xlsx</t>
-  </si>
-  <si>
-    <t>0p3_RhNP_0p0204_500C_20250315_PSULeft.xlsx</t>
-  </si>
-  <si>
     <t>Rh %</t>
   </si>
   <si>
@@ -228,6 +132,102 @@
   </si>
   <si>
     <t>400</t>
+  </si>
+  <si>
+    <t>2p0_RhWI_0p02_500C_20250331_LaboratoryA_Right.xlsx</t>
+  </si>
+  <si>
+    <t>2_RhWI_0p027_600C_20250422_LaboratoryA_Right.xlsx</t>
+  </si>
+  <si>
+    <t>0p3_RhWI_0p0207_500C_20250315_LaboratoryA_Right.xlsx</t>
+  </si>
+  <si>
+    <t>0p1_RhWI_0p02_500C_20250414_LaboratoryA_Right.xlsx</t>
+  </si>
+  <si>
+    <t>2_RhWI_0p01824_500C_20250401_LaboratoryA_Right.xlsx</t>
+  </si>
+  <si>
+    <t>2_RhWI_0p021_400C_20250425_LaboratoryA_Right.xlsx</t>
+  </si>
+  <si>
+    <t>2_RhWI_0p02_500C_20250403_LaboratoryA_Right.xlsx</t>
+  </si>
+  <si>
+    <t>0p3_RhNP_0p0204_500C_20250315_LaboratoryA_Left.xlsx</t>
+  </si>
+  <si>
+    <t>0p3_RhWI_0p02mg_500C_20250331_LaboratoryB_.xlsx</t>
+  </si>
+  <si>
+    <t>0p3_RhWI_0p0199mg_500C_20250415_LaboratoryB_.xlsx</t>
+  </si>
+  <si>
+    <t>0p3_RhWI_0p0204mg_500C_20250421_LaboratoryB_.xlsx</t>
+  </si>
+  <si>
+    <t>2_RhWI_0p02mg_400C_20250422_LaboratoryB_.xlsx</t>
+  </si>
+  <si>
+    <t>2_RhWI_0p02mg_500C_20250417_LaboratoryB_.xlsx</t>
+  </si>
+  <si>
+    <t>0p1_RhWI_0p02mg_500C_20250418_LaboratoryB_.xlsx</t>
+  </si>
+  <si>
+    <t>2_RhWI_0p02mg_600C_20250423_LaboratoryB_.xlsx</t>
+  </si>
+  <si>
+    <t>0p3_RhNP_0p0201mg_500C_20250424_LaboratoryB_.xlsx</t>
+  </si>
+  <si>
+    <t>0p1_RhWI_0p02mg_500C_20250319_LaboratoryC_RR.xlsx</t>
+  </si>
+  <si>
+    <t>0p3_RhNP_0p0201mg_500C_20250312_LaboratoryC_RR.xlsx</t>
+  </si>
+  <si>
+    <t>0p3_RhWI_0p0201mg_500C_20250311_LaboratoryC_RR.xlsx</t>
+  </si>
+  <si>
+    <t>2_RhWI_0p02mg_400C_20250306_LaboratoryC_RR.xlsx</t>
+  </si>
+  <si>
+    <t>2_RhWI_0p02mg_600C_20250318_LaboratoryC_RR.xlsx</t>
+  </si>
+  <si>
+    <t>2_RhWI_0p02mg_500C_20250307_LaboratoryC_RR.xlsx</t>
+  </si>
+  <si>
+    <t>0p1_RhWI_0p02mg_500C_20250314_LaboratoryC_RR.xlsx</t>
+  </si>
+  <si>
+    <t>0p1_RhWI_0p02mg_500C_20250317_LaboratoryC_RR.xlsx</t>
+  </si>
+  <si>
+    <t>0p3_RhNP_0p0197mg_500C_20250211_LaboratoryD_.xlsx</t>
+  </si>
+  <si>
+    <t>2_RhWI_0p0202mg_500C_20250317_LaboratoryD_.xlsx</t>
+  </si>
+  <si>
+    <t>0p3_RhWI_0p02mg_500C_20250312_LaboratoryD_.xlsx</t>
+  </si>
+  <si>
+    <t>2_RhWI_0p0204mg_400C_20250324_LaboratoryD_.xlsx</t>
+  </si>
+  <si>
+    <t>0p3_RhNP_0p0201mg_500C_20250207_LaboratoryD_.xlsx</t>
+  </si>
+  <si>
+    <t>2_RhWI_0p02mg_600C_20250326_LaboratoryD_.xlsx</t>
+  </si>
+  <si>
+    <t>0p1_RhWI_0p02mg_500C_20250314_LaboratoryD_.xlsx</t>
+  </si>
+  <si>
+    <t>0p3_RhNP_0p0199mg_500C_20250212_LaboratoryD_.xlsx</t>
   </si>
 </sst>
 </file>
@@ -594,7 +594,7 @@
   <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -607,13 +607,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -690,16 +690,16 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <v>41.702440773746289</v>
@@ -776,16 +776,16 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B3">
         <v>0.3</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E3">
         <v>22.140354049769648</v>
@@ -862,16 +862,16 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>0.3</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E4">
         <v>33.271954881300132</v>
@@ -948,16 +948,16 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E5">
         <v>14.71762536872772</v>
@@ -1034,16 +1034,16 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>0.3</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E6">
         <v>37.778253260826382</v>
@@ -1120,16 +1120,16 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E7">
         <v>32.086915669981849</v>
@@ -1206,16 +1206,16 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>0.3</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E8">
         <v>35.699563100433423</v>
@@ -1292,16 +1292,16 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="E9">
         <v>55.654446759591544</v>
@@ -1378,16 +1378,16 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>0.3</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E10">
         <v>44.58465411482085</v>
@@ -1464,16 +1464,16 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E11">
         <v>8.5223770525322617</v>
@@ -1550,16 +1550,16 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B12">
         <v>0.3</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E12">
         <v>19.529579325384191</v>
@@ -1636,16 +1636,16 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B13">
         <v>0.3</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E13">
         <v>42.708820675165391</v>
@@ -1722,16 +1722,16 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E14">
         <v>26.18609633329794</v>
@@ -1808,16 +1808,16 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E15">
         <v>11.003274133231139</v>
@@ -1894,16 +1894,16 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B16">
         <v>0.3</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E16">
         <v>38.824272770361702</v>
@@ -1980,16 +1980,16 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="B17">
         <v>0.3</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E17">
         <v>21.529527314816718</v>
@@ -2066,16 +2066,16 @@
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E18">
         <v>10.390277571674449</v>
@@ -2152,16 +2152,16 @@
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>0.1</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E19">
         <v>17.157432484190171</v>
@@ -2238,16 +2238,16 @@
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <v>40.73675738764554</v>
@@ -2324,16 +2324,16 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E21">
         <v>25.106679790437958</v>
@@ -2410,16 +2410,16 @@
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B22">
         <v>0.1</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E22">
         <v>23.102227391190951</v>
@@ -2496,16 +2496,16 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="E23">
         <v>34.311706489636528</v>
@@ -2582,16 +2582,16 @@
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E24">
         <v>38.869522689336193</v>
@@ -2668,16 +2668,16 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="E25">
         <v>20.80784877339504</v>
@@ -2754,16 +2754,16 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B26">
         <v>0.1</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E26">
         <v>14.694959143186789</v>
@@ -2840,16 +2840,16 @@
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B27">
         <v>0.1</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E27">
         <v>22.588124421079289</v>
@@ -2926,16 +2926,16 @@
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B28">
         <v>0.3</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E28">
         <v>14.15978971576785</v>
@@ -3012,16 +3012,16 @@
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B29">
         <v>0.1</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E29">
         <v>15.561184369286471</v>
@@ -3098,16 +3098,16 @@
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E30">
         <v>14.626497526224989</v>
@@ -3184,16 +3184,16 @@
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E31">
         <v>42.026062785844474</v>
@@ -3270,16 +3270,16 @@
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B32">
         <v>0.3</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E32">
         <v>19.78733994110047</v>
@@ -3356,16 +3356,16 @@
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B33">
         <v>0.3</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E33">
         <v>22.693115674893111</v>

</xml_diff>